<commit_message>
Number values get their .0 removed
</commit_message>
<xml_diff>
--- a/_testdata/Worksheet1.xlsx
+++ b/_testdata/Worksheet1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="4960" yWindow="2000" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I87" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -463,6 +463,9 @@
       </c>
     </row>
     <row r="2" spans="1:29">
+      <c r="D2">
+        <v>4</v>
+      </c>
       <c r="AA2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Strip \r in multi-line cells
I was unable to reproduce the problem, but I had
a table that contained these values that should
be removed.
</commit_message>
<xml_diff>
--- a/_testdata/Worksheet1.xlsx
+++ b/_testdata/Worksheet1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="4960" yWindow="2000" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>A</t>
   </si>
@@ -41,6 +41,10 @@
   </si>
   <si>
     <t>row101</t>
+  </si>
+  <si>
+    <t>a
+b</t>
   </si>
 </sst>
 </file>
@@ -53,7 +57,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -92,18 +95,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,10 +446,13 @@
   <dimension ref="A1:AC101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" t="s">
@@ -480,6 +493,11 @@
       <c r="C3">
         <f>B3*2</f>
         <v>246.91200000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="45">
+      <c r="E5" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:29">

</xml_diff>

<commit_message>
Bugfix for table cells with formatting
When table cells have more than one formatting, the string could
be split in multiple pieces. 

See https://docs.microsoft.com/de-de/office/open-xml/working-with-the-shared-string-table
</commit_message>
<xml_diff>
--- a/_testdata/Worksheet1.xlsx
+++ b/_testdata/Worksheet1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="4960" yWindow="2000" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>A</t>
   </si>
@@ -45,18 +45,35 @@
   <si>
     <t>a
 b</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Some </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>text</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -75,6 +92,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -446,7 +471,7 @@
   <dimension ref="A1:AC101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -496,6 +521,9 @@
       </c>
     </row>
     <row r="5" spans="1:29" ht="45">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>